<commit_message>
Fit inflammation and add positive feedback in dI & before LHS
</commit_message>
<xml_diff>
--- a/detailed_model_2/FitIAV/data_to_fit.xlsx
+++ b/detailed_model_2/FitIAV/data_to_fit.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14040" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14040" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="105">
   <si>
     <t>CD45 cells (as % of all live cells)</t>
   </si>
@@ -444,12 +445,224 @@
     <t>Mono</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Relation between weight change and survival curve</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dpi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weight change</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>survival ratio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fig1b. flu_ZT23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fig1b. flu_ZT11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fig1f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Bmal1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>fl/fl</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ErCre</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(ZT23)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Bmal1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>fl/fl</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ErCre</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(ZT11)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Bmal1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>fl/fl</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ErCre</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(ZT23)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Bmal1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>fl/fl</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ErCre</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(ZT11)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,6 +748,36 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -779,7 +1022,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -956,6 +1199,21 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1239,16 +1497,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA121"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -1266,7 +1524,7 @@
       <c r="O1" s="69"/>
       <c r="P1" s="69"/>
     </row>
-    <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="63" t="s">
         <v>1</v>
@@ -1286,7 +1544,7 @@
       <c r="O2" s="70"/>
       <c r="P2" s="70"/>
     </row>
-    <row r="3" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1316,7 +1574,7 @@
       <c r="O3" s="69"/>
       <c r="P3" s="69"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -1346,7 +1604,7 @@
       <c r="O4" s="70"/>
       <c r="P4" s="70"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -1376,7 +1634,7 @@
       <c r="O5" s="70"/>
       <c r="P5" s="70"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -1399,7 +1657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -1422,7 +1680,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="40"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1431,7 +1689,7 @@
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="41" t="s">
         <v>69</v>
       </c>
@@ -1469,7 +1727,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="66" t="s">
         <v>1</v>
@@ -1508,7 +1766,7 @@
         <v>9.2563999999999993</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="42" t="s">
         <v>3</v>
       </c>
@@ -1557,7 +1815,7 @@
         <v>44.036639999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>1</v>
       </c>
@@ -1606,7 +1864,7 @@
         <v>72.287599999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>2</v>
       </c>
@@ -1655,7 +1913,7 @@
         <v>157.34399999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>4</v>
       </c>
@@ -1704,7 +1962,7 @@
         <v>19.006</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>6</v>
       </c>
@@ -1753,7 +2011,7 @@
         <v>123.4286</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="40"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1788,7 +2046,7 @@
         <v>150.44199999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="30" t="s">
         <v>12</v>
       </c>
@@ -1829,7 +2087,7 @@
         <v>81.224999999999994</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="63" t="s">
         <v>1</v>
@@ -1848,7 +2106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
@@ -1877,7 +2135,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>1</v>
       </c>
@@ -1908,7 +2166,7 @@
         <v>2.7864</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="18">
         <v>2</v>
       </c>
@@ -1939,7 +2197,7 @@
         <v>14.855300000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>4</v>
       </c>
@@ -1970,7 +2228,7 @@
         <v>16.263999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>6</v>
       </c>
@@ -2001,7 +2259,7 @@
         <v>18.468</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="30" t="s">
         <v>13</v>
       </c>
@@ -2016,7 +2274,7 @@
       </c>
       <c r="I25" s="30"/>
     </row>
-    <row r="26" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="63" t="s">
         <v>1</v>
@@ -2035,7 +2293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
@@ -2064,7 +2322,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="18">
         <v>1</v>
       </c>
@@ -2095,7 +2353,7 @@
         <v>11.1456</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="18">
         <v>2</v>
       </c>
@@ -2126,7 +2384,7 @@
         <v>2.7863000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="18">
         <v>4</v>
       </c>
@@ -2157,7 +2415,7 @@
         <v>3.8000000000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="19">
         <v>6</v>
       </c>
@@ -2188,7 +2446,7 @@
         <v>2.3328000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="30" t="s">
         <v>14</v>
       </c>
@@ -2203,7 +2461,7 @@
       </c>
       <c r="I33" s="30"/>
     </row>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
       <c r="B34" s="63" t="s">
         <v>1</v>
@@ -2222,7 +2480,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22" t="s">
         <v>3</v>
       </c>
@@ -2251,7 +2509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="23">
         <v>1</v>
       </c>
@@ -2282,7 +2540,7 @@
         <v>4.0823999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="27">
         <v>2</v>
       </c>
@@ -2313,7 +2571,7 @@
         <v>9.1635000000000009</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="27">
         <v>4</v>
       </c>
@@ -2344,7 +2602,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="28">
         <v>6</v>
       </c>
@@ -2378,7 +2636,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="38"/>
       <c r="B40" s="38"/>
       <c r="C40" s="38"/>
@@ -2387,7 +2645,7 @@
       <c r="F40" s="38"/>
       <c r="G40" s="38"/>
     </row>
-    <row r="41" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="30" t="s">
         <v>15</v>
       </c>
@@ -2402,7 +2660,7 @@
       </c>
       <c r="I41" s="30"/>
     </row>
-    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14"/>
       <c r="B42" s="66" t="s">
         <v>1</v>
@@ -2421,7 +2679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>3</v>
       </c>
@@ -2450,7 +2708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="18">
         <v>1</v>
       </c>
@@ -2481,7 +2739,7 @@
         <v>1.0368000000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="18">
         <v>2</v>
       </c>
@@ -2512,7 +2770,7 @@
         <v>0.60345000000000004</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="18">
         <v>4</v>
       </c>
@@ -2543,7 +2801,7 @@
         <v>1.1856</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <v>6</v>
       </c>
@@ -2574,7 +2832,7 @@
         <v>0.58320000000000005</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="38"/>
       <c r="B48" s="38"/>
       <c r="C48" s="38"/>
@@ -2583,7 +2841,7 @@
       <c r="F48" s="38"/>
       <c r="G48" s="38"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="38"/>
       <c r="B49" s="38"/>
       <c r="C49" s="38"/>
@@ -2592,7 +2850,7 @@
       <c r="F49" s="38"/>
       <c r="G49" s="38"/>
     </row>
-    <row r="50" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="30" t="s">
         <v>16</v>
       </c>
@@ -2607,7 +2865,7 @@
       </c>
       <c r="I50" s="30"/>
     </row>
-    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="14"/>
       <c r="B51" s="63" t="s">
         <v>1</v>
@@ -2626,7 +2884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>3</v>
       </c>
@@ -2655,7 +2913,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="18">
         <v>1</v>
       </c>
@@ -2686,7 +2944,7 @@
         <v>0.9071999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="18">
         <v>2</v>
       </c>
@@ -2717,7 +2975,7 @@
         <v>1.30375</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="18">
         <v>4</v>
       </c>
@@ -2748,7 +3006,7 @@
         <v>5.548</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="19">
         <v>6</v>
       </c>
@@ -2779,7 +3037,7 @@
         <v>3.1103999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="47"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -2790,7 +3048,7 @@
       <c r="H57" s="48"/>
       <c r="I57" s="48"/>
     </row>
-    <row r="58" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="41" t="s">
         <v>78</v>
       </c>
@@ -2803,7 +3061,7 @@
       <c r="H58" s="48"/>
       <c r="I58" s="48"/>
     </row>
-    <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="14"/>
       <c r="B59" s="63" t="s">
         <v>1</v>
@@ -2818,7 +3076,7 @@
       <c r="H59" s="48"/>
       <c r="I59" s="48"/>
     </row>
-    <row r="60" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>3</v>
       </c>
@@ -2843,7 +3101,7 @@
       <c r="H60" s="48"/>
       <c r="I60" s="48"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="18">
         <v>1</v>
       </c>
@@ -2868,7 +3126,7 @@
       <c r="H61" s="48"/>
       <c r="I61" s="48"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="18">
         <v>2</v>
       </c>
@@ -2893,7 +3151,7 @@
       <c r="H62" s="48"/>
       <c r="I62" s="48"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="18">
         <v>4</v>
       </c>
@@ -2918,7 +3176,7 @@
       <c r="H63" s="48"/>
       <c r="I63" s="48"/>
     </row>
-    <row r="64" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="19">
         <v>6</v>
       </c>
@@ -2943,7 +3201,7 @@
       <c r="H64" s="48"/>
       <c r="I64" s="48"/>
     </row>
-    <row r="66" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="30" t="s">
         <v>17</v>
       </c>
@@ -2958,7 +3216,7 @@
       </c>
       <c r="I66" s="30"/>
     </row>
-    <row r="67" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="29"/>
       <c r="B67" s="63" t="s">
         <v>1</v>
@@ -2977,7 +3235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>3</v>
       </c>
@@ -3006,7 +3264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="18">
         <v>1</v>
       </c>
@@ -3037,7 +3295,7 @@
         <v>6.2207999999999997</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="18">
         <v>2</v>
       </c>
@@ -3068,7 +3326,7 @@
         <v>4.8201499999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="18">
         <v>4</v>
       </c>
@@ -3099,7 +3357,7 @@
         <v>7.1440000000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="19">
         <v>6</v>
       </c>
@@ -3130,12 +3388,12 @@
         <v>7.7759999999999989</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="31" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="31" t="s">
         <v>19</v>
       </c>
@@ -3146,7 +3404,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="39" t="s">
         <v>20</v>
       </c>
@@ -3157,7 +3415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
         <v>21</v>
       </c>
@@ -3168,7 +3426,7 @@
         <v>2.0249999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="39" t="s">
         <v>22</v>
       </c>
@@ -3179,7 +3437,7 @@
         <v>5.1749999999999998</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="39" t="s">
         <v>23</v>
       </c>
@@ -3190,7 +3448,7 @@
         <v>4.7750000000000004</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="39" t="s">
         <v>24</v>
       </c>
@@ -3201,7 +3459,7 @@
         <v>5.6749999999999998</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="39" t="s">
         <v>25</v>
       </c>
@@ -3212,7 +3470,7 @@
         <v>4.6500000000000004</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="39" t="s">
         <v>26</v>
       </c>
@@ -3223,7 +3481,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="39" t="s">
         <v>27</v>
       </c>
@@ -3234,7 +3492,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="31" t="s">
         <v>41</v>
       </c>
@@ -3254,7 +3512,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="31" t="s">
         <v>38</v>
       </c>
@@ -3276,7 +3534,7 @@
         <v>135.5384</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="31" t="s">
         <v>39</v>
       </c>
@@ -3298,7 +3556,7 @@
         <v>202.28825000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="31" t="s">
         <v>52</v>
       </c>
@@ -3318,7 +3576,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="31" t="s">
         <v>40</v>
       </c>
@@ -3340,7 +3598,7 @@
         <v>110.23039999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="31" t="s">
         <v>39</v>
       </c>
@@ -3362,7 +3620,7 @@
         <v>164.50200000000001</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="31" t="s">
         <v>86</v>
       </c>
@@ -3370,7 +3628,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B94" s="31" t="s">
         <v>28</v>
       </c>
@@ -3389,7 +3647,7 @@
         <v>25.308000000000007</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="31" t="s">
         <v>42</v>
       </c>
@@ -3413,7 +3671,7 @@
         <v>37.786249999999995</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="31" t="s">
         <v>43</v>
       </c>
@@ -3426,12 +3684,12 @@
         <v>18.6462</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" s="31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B99" s="31" t="s">
         <v>45</v>
       </c>
@@ -3439,7 +3697,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" s="31" t="s">
         <v>47</v>
       </c>
@@ -3452,7 +3710,7 @@
         <v>10.160639999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" s="31" t="s">
         <v>48</v>
       </c>
@@ -3465,12 +3723,12 @@
         <v>15.1632</v>
       </c>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" s="31" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B104" s="31" t="s">
         <v>8</v>
       </c>
@@ -3478,7 +3736,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" s="31" t="s">
         <v>42</v>
       </c>
@@ -3491,7 +3749,7 @@
         <v>2.3328000000000024</v>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" s="31" t="s">
         <v>43</v>
       </c>
@@ -3504,7 +3762,7 @@
         <v>3.4830000000000005</v>
       </c>
     </row>
-    <row r="109" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="52" t="s">
         <v>79</v>
       </c>
@@ -3533,7 +3791,7 @@
       <c r="X109" s="53"/>
       <c r="Y109" s="53"/>
     </row>
-    <row r="110" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="54"/>
       <c r="B110" s="60" t="s">
         <v>1</v>
@@ -3570,7 +3828,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" s="18">
         <v>1</v>
       </c>
@@ -3625,7 +3883,7 @@
         <v>6.1480000000000006</v>
       </c>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" s="18">
         <v>2</v>
       </c>
@@ -3682,7 +3940,7 @@
         <v>102.06399999999999</v>
       </c>
     </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A113" s="18">
         <v>4</v>
       </c>
@@ -3759,7 +4017,7 @@
         <v>693.57800000000009</v>
       </c>
     </row>
-    <row r="114" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:27" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="19">
         <v>6</v>
       </c>
@@ -3844,10 +4102,10 @@
         <v>1090.0008333333335</v>
       </c>
     </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
       <c r="AA115" s="48"/>
     </row>
-    <row r="116" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="52" t="s">
         <v>80</v>
       </c>
@@ -3878,7 +4136,7 @@
       <c r="Z116" s="52"/>
       <c r="AA116" s="48"/>
     </row>
-    <row r="117" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="55"/>
       <c r="B117" s="60" t="s">
         <v>1</v>
@@ -3915,7 +4173,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="118" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A118" s="18">
         <v>1</v>
       </c>
@@ -3970,7 +4228,7 @@
         <v>17.032</v>
       </c>
     </row>
-    <row r="119" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A119" s="18">
         <v>2</v>
       </c>
@@ -4027,7 +4285,7 @@
         <v>178.74600000000001</v>
       </c>
     </row>
-    <row r="120" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A120" s="18">
         <v>4</v>
       </c>
@@ -4104,7 +4362,7 @@
         <v>1284.3119999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:27" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="19">
         <v>6</v>
       </c>
@@ -4227,12 +4485,12 @@
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>32</v>
       </c>
@@ -4249,7 +4507,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>31</v>
       </c>
@@ -4266,7 +4524,7 @@
         <v>40.158839999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>30</v>
       </c>
@@ -4283,7 +4541,7 @@
         <v>9.3234000000000012</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>32</v>
       </c>
@@ -4314,7 +4572,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>33</v>
       </c>
@@ -4343,7 +4601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>34</v>
       </c>
@@ -4368,7 +4626,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>35</v>
       </c>
@@ -4391,7 +4649,7 @@
         <v>3.6068164140000007</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>36</v>
       </c>
@@ -4414,7 +4672,7 @@
         <v>19.133183586000001</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>49</v>
       </c>
@@ -4431,7 +4689,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>31</v>
       </c>
@@ -4448,7 +4706,7 @@
         <v>33.307200000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
         <v>30</v>
       </c>
@@ -4465,7 +4723,7 @@
         <v>7.7759999999999989</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>50</v>
       </c>
@@ -4496,7 +4754,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>33</v>
       </c>
@@ -4525,7 +4783,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>51</v>
       </c>
@@ -4550,7 +4808,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>35</v>
       </c>
@@ -4573,7 +4831,7 @@
         <v>3.4830000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>36</v>
       </c>
@@ -4607,16 +4865,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>85</v>
       </c>
@@ -4633,7 +4891,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>54</v>
       </c>
@@ -4650,7 +4908,7 @@
         <v>190.27968337730874</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>9</v>
       </c>
@@ -4667,7 +4925,7 @@
         <v>154.81481481481481</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>56</v>
       </c>
@@ -4684,7 +4942,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>54</v>
       </c>
@@ -4701,7 +4959,7 @@
         <v>26.224</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>9</v>
       </c>
@@ -4718,7 +4976,7 @@
         <v>10.26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>93</v>
       </c>
@@ -4735,7 +4993,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>8</v>
       </c>
@@ -4752,7 +5010,7 @@
         <v>157.34399999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>9</v>
       </c>
@@ -4769,7 +5027,7 @@
         <v>81.224999999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>62</v>
       </c>
@@ -4786,7 +5044,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>54</v>
       </c>
@@ -4803,7 +5061,7 @@
         <v>99.531999999999982</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
         <v>9</v>
       </c>
@@ -4820,7 +5078,7 @@
         <v>38.76</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>55</v>
       </c>
@@ -4837,7 +5095,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>8</v>
       </c>
@@ -4854,7 +5112,7 @@
         <v>70.3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>9</v>
       </c>
@@ -4871,7 +5129,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>53</v>
       </c>
@@ -4902,7 +5160,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>54</v>
       </c>
@@ -4931,7 +5189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>57</v>
       </c>
@@ -4960,7 +5218,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>58</v>
       </c>
@@ -4985,7 +5243,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>54</v>
       </c>
@@ -5008,7 +5266,7 @@
         <v>33.451080990000008</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>57</v>
       </c>
@@ -5031,7 +5289,7 @@
         <v>37.786249999999995</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>59</v>
       </c>
@@ -5056,7 +5314,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>54</v>
       </c>
@@ -5079,7 +5337,7 @@
         <v>177.44891901</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>57</v>
       </c>
@@ -5102,7 +5360,7 @@
         <v>164.50200000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
         <v>60</v>
       </c>
@@ -5119,7 +5377,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
         <v>54</v>
       </c>
@@ -5136,7 +5394,7 @@
         <v>1400.1125000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
         <v>57</v>
       </c>
@@ -5153,7 +5411,7 @@
         <v>1090.0008333333335</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>61</v>
       </c>
@@ -5170,7 +5428,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>54</v>
       </c>
@@ -5187,7 +5445,7 @@
         <v>3290.3127272727274</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>57</v>
       </c>
@@ -5209,4 +5467,739 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="71"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="E4" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2.06</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>-1.7</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>-0.52</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>1.2</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>-0.53</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>-2.5</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>-4.4400000000000004</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>-10.86</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>-8.73</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>-12.73</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>-8.1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>-17.27</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>-15.2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>-20.61</v>
+      </c>
+      <c r="G12">
+        <f>18/24</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>-17.5</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>-23.61</v>
+      </c>
+      <c r="G13">
+        <f>16/24</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>-17</v>
+      </c>
+      <c r="C14">
+        <f>19/20</f>
+        <v>0.95</v>
+      </c>
+      <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="F14">
+        <v>-21.27</v>
+      </c>
+      <c r="G14">
+        <f>9/24</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>-16.03</v>
+      </c>
+      <c r="C15">
+        <f>18/20</f>
+        <v>0.9</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15">
+        <v>-21.16</v>
+      </c>
+      <c r="G15">
+        <f>8/24</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>-8.7200000000000006</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:C18" si="0">18/20</f>
+        <v>0.9</v>
+      </c>
+      <c r="E16">
+        <v>11</v>
+      </c>
+      <c r="F16">
+        <v>-17.07</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16:G18" si="1">8/24</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>-6.42</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="E17">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>-19.579999999999998</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>-2.4900000000000002</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="E18">
+        <v>13</v>
+      </c>
+      <c r="F18">
+        <v>-10.61</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>-1.22</v>
+      </c>
+      <c r="C19">
+        <f>17/20</f>
+        <v>0.85</v>
+      </c>
+      <c r="E19">
+        <v>14</v>
+      </c>
+      <c r="F19">
+        <v>-7.79</v>
+      </c>
+      <c r="G19">
+        <f>7/24</f>
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="73" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="74"/>
+      <c r="C22" s="75"/>
+      <c r="E22" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="I22" s="73" t="s">
+        <v>103</v>
+      </c>
+      <c r="J22" s="74"/>
+      <c r="K22" s="75"/>
+      <c r="M22" s="73" t="s">
+        <v>104</v>
+      </c>
+      <c r="N22" s="74"/>
+      <c r="O22" s="75"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" t="s">
+        <v>97</v>
+      </c>
+      <c r="I23" t="s">
+        <v>95</v>
+      </c>
+      <c r="J23" t="s">
+        <v>96</v>
+      </c>
+      <c r="K23" t="s">
+        <v>97</v>
+      </c>
+      <c r="M23" t="s">
+        <v>95</v>
+      </c>
+      <c r="N23" t="s">
+        <v>96</v>
+      </c>
+      <c r="O23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1.9</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1.17</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1.6</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>-2.5499999999999998</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>-1.07</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25">
+        <v>-3.43</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>2</v>
+      </c>
+      <c r="N25">
+        <v>-2.1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>-6.5</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>-7.2</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <v>-9.0500000000000007</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>3</v>
+      </c>
+      <c r="N26">
+        <v>-10.3</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>-9.4</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>-12.13</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>4</v>
+      </c>
+      <c r="J27">
+        <v>-13.2</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>4</v>
+      </c>
+      <c r="N27">
+        <v>-13.2</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>-11.6</v>
+      </c>
+      <c r="C28">
+        <f>46/47</f>
+        <v>0.97872340425531912</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <v>-15.14</v>
+      </c>
+      <c r="G28">
+        <f>39/41</f>
+        <v>0.95121951219512191</v>
+      </c>
+      <c r="I28">
+        <v>5</v>
+      </c>
+      <c r="J28">
+        <v>-16.23</v>
+      </c>
+      <c r="K28">
+        <f>12/13</f>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="M28">
+        <v>5</v>
+      </c>
+      <c r="N28">
+        <v>-9.74</v>
+      </c>
+      <c r="O28">
+        <f>11/12</f>
+        <v>0.91666666666666663</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>-11.04</v>
+      </c>
+      <c r="C29">
+        <f>39/47</f>
+        <v>0.82978723404255317</v>
+      </c>
+      <c r="E29">
+        <v>6</v>
+      </c>
+      <c r="F29">
+        <v>-19.2</v>
+      </c>
+      <c r="G29">
+        <f>34/41</f>
+        <v>0.82926829268292679</v>
+      </c>
+      <c r="I29">
+        <v>6</v>
+      </c>
+      <c r="J29">
+        <v>-15.7</v>
+      </c>
+      <c r="K29">
+        <f>12/13</f>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="M29">
+        <v>6</v>
+      </c>
+      <c r="N29">
+        <v>-16.2</v>
+      </c>
+      <c r="O29">
+        <f>9/12</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <v>-13.5</v>
+      </c>
+      <c r="C30">
+        <f>35/47</f>
+        <v>0.74468085106382975</v>
+      </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30">
+        <v>-23.5</v>
+      </c>
+      <c r="G30">
+        <f>26/41</f>
+        <v>0.63414634146341464</v>
+      </c>
+      <c r="I30">
+        <v>7</v>
+      </c>
+      <c r="J30">
+        <v>-21.9</v>
+      </c>
+      <c r="K30">
+        <f>7/13</f>
+        <v>0.53846153846153844</v>
+      </c>
+      <c r="M30">
+        <v>7</v>
+      </c>
+      <c r="N30">
+        <v>-22.2</v>
+      </c>
+      <c r="O30">
+        <f>9/12</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>8</v>
+      </c>
+      <c r="B31">
+        <v>-16.2</v>
+      </c>
+      <c r="C31">
+        <f>34/47</f>
+        <v>0.72340425531914898</v>
+      </c>
+      <c r="E31">
+        <v>8</v>
+      </c>
+      <c r="F31">
+        <v>-23.5</v>
+      </c>
+      <c r="G31">
+        <f>19/41</f>
+        <v>0.46341463414634149</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="E22:G22"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>